<commit_message>
updated merged data with accurate power consumption
</commit_message>
<xml_diff>
--- a/Resources/US_Population_2000_to_2010.xlsx
+++ b/Resources/US_Population_2000_to_2010.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d9339f47db2de4a/Desktop/GitHub Repo/DataSci HW Submittal/Project-1/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\OneDrive\MyDocuments\Education\GaTech\DataScience\publishedHW\Project-1\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC07BF71-9B21-49A2-8372-3A4BDE5917D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FC07BF71-9B21-49A2-8372-3A4BDE5917D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BFCC966-06E7-4D9D-AC4B-01CA0E93CB06}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{856DEAD3-037E-4537-8B0B-2C8D0DBF9BF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{856DEAD3-037E-4537-8B0B-2C8D0DBF9BF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,16 +610,16 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="10.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -695,7 +695,7 @@
         <v>309349689</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -733,7 +733,7 @@
         <v>4785298</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -771,7 +771,7 @@
         <v>713985</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -809,7 +809,7 @@
         <v>6413737</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -847,7 +847,7 @@
         <v>2921606</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -885,7 +885,7 @@
         <v>37349363</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -923,7 +923,7 @@
         <v>5049071</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -961,7 +961,7 @@
         <v>3577073</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -999,7 +999,7 @@
         <v>899769</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>604453</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>18843326</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>9712587</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>1363621</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>1571450</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>12843166</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>6490621</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>3049883</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>2859169</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>4346266</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>4544228</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>1327567</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>5785982</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>6557254</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>9877574</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>5310584</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>2970036</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>5996231</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>990898</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>1830429</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>2704642</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1316759</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>8801624</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>2065932</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>19392283</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>9561558</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>674499</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>11536182</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>3761702</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>3838957</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>12709630</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>41</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>1052886</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>4636312</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>43</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>816463</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>44</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>6356897</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>25257114</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>2776469</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>625960</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>8024617</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>49</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>6744496</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>1853973</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>51</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>5691047</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Pushing Population data/file updates
</commit_message>
<xml_diff>
--- a/Resources/US_Population_2000_to_2010.xlsx
+++ b/Resources/US_Population_2000_to_2010.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d9339f47db2de4a/Desktop/GitHub Repo/DataSci HW Submittal/Project-1/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XxTopShottAxX\OneDrive\Desktop\GitHub Repo\DataSci HW Submittal\Project-1\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC07BF71-9B21-49A2-8372-3A4BDE5917D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FC07BF71-9B21-49A2-8372-3A4BDE5917D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC806CEA-3B20-4EEF-BD74-3A8127C895AB}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{856DEAD3-037E-4537-8B0B-2C8D0DBF9BF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateCount="1000" calcOnSave="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Geographic Area</t>
   </si>
@@ -190,13 +191,178 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Population Change</t>
+  </si>
+  <si>
+    <t>state,area (sq. mi)</t>
+  </si>
+  <si>
+    <t>Alabama,52423</t>
+  </si>
+  <si>
+    <t>Alaska,656425</t>
+  </si>
+  <si>
+    <t>Arizona,114006</t>
+  </si>
+  <si>
+    <t>Arkansas,53182</t>
+  </si>
+  <si>
+    <t>California,163707</t>
+  </si>
+  <si>
+    <t>Colorado,104100</t>
+  </si>
+  <si>
+    <t>Connecticut,5544</t>
+  </si>
+  <si>
+    <t>Delaware,1954</t>
+  </si>
+  <si>
+    <t>Florida,65758</t>
+  </si>
+  <si>
+    <t>Georgia,59441</t>
+  </si>
+  <si>
+    <t>Hawaii,10932</t>
+  </si>
+  <si>
+    <t>Idaho,83574</t>
+  </si>
+  <si>
+    <t>Illinois,57918</t>
+  </si>
+  <si>
+    <t>Indiana,36420</t>
+  </si>
+  <si>
+    <t>Iowa,56276</t>
+  </si>
+  <si>
+    <t>Kansas,82282</t>
+  </si>
+  <si>
+    <t>Kentucky,40411</t>
+  </si>
+  <si>
+    <t>Louisiana,51843</t>
+  </si>
+  <si>
+    <t>Maine,35387</t>
+  </si>
+  <si>
+    <t>Maryland,12407</t>
+  </si>
+  <si>
+    <t>Massachusetts,10555</t>
+  </si>
+  <si>
+    <t>Michigan,96810</t>
+  </si>
+  <si>
+    <t>Minnesota,86943</t>
+  </si>
+  <si>
+    <t>Mississippi,48434</t>
+  </si>
+  <si>
+    <t>Missouri,69709</t>
+  </si>
+  <si>
+    <t>Montana,147046</t>
+  </si>
+  <si>
+    <t>Nebraska,77358</t>
+  </si>
+  <si>
+    <t>Nevada,110567</t>
+  </si>
+  <si>
+    <t>New Hampshire,9351</t>
+  </si>
+  <si>
+    <t>New Jersey,8722</t>
+  </si>
+  <si>
+    <t>New Mexico,121593</t>
+  </si>
+  <si>
+    <t>New York,54475</t>
+  </si>
+  <si>
+    <t>North Carolina,53821</t>
+  </si>
+  <si>
+    <t>North Dakota,70704</t>
+  </si>
+  <si>
+    <t>Ohio,44828</t>
+  </si>
+  <si>
+    <t>Oklahoma,69903</t>
+  </si>
+  <si>
+    <t>Oregon,98386</t>
+  </si>
+  <si>
+    <t>Pennsylvania,46058</t>
+  </si>
+  <si>
+    <t>Rhode Island,1545</t>
+  </si>
+  <si>
+    <t>South Carolina,32007</t>
+  </si>
+  <si>
+    <t>South Dakota,77121</t>
+  </si>
+  <si>
+    <t>Tennessee,42146</t>
+  </si>
+  <si>
+    <t>Texas,268601</t>
+  </si>
+  <si>
+    <t>Utah,84904</t>
+  </si>
+  <si>
+    <t>Vermont,9615</t>
+  </si>
+  <si>
+    <t>Virginia,42769</t>
+  </si>
+  <si>
+    <t>Washington,71303</t>
+  </si>
+  <si>
+    <t>West Virginia,24231</t>
+  </si>
+  <si>
+    <t>Wisconsin,65503</t>
+  </si>
+  <si>
+    <t>Wyoming,97818</t>
+  </si>
+  <si>
+    <t>District of Columbia,68</t>
+  </si>
+  <si>
+    <t>Puerto Rico,3515</t>
+  </si>
+  <si>
+    <t>Area (Sq. Mi)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +375,11 @@
       <sz val="10"/>
       <name val="MS Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -268,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,6 +463,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,19 +781,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1E7B0F-380B-466D-BDF0-60538CBCE175}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="10.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="10.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" ht="24.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,8 +830,14 @@
       <c r="L1" s="2">
         <v>2010</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -694,8 +874,16 @@
       <c r="L2" s="4">
         <v>309349689</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M2" s="4">
+        <f>L2-B2</f>
+        <v>27187278</v>
+      </c>
+      <c r="N2" s="4">
+        <f>SUM(N3:N53)</f>
+        <v>3786884</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -732,8 +920,15 @@
       <c r="L3" s="6">
         <v>4785298</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M3" s="6">
+        <f t="shared" ref="M3:M53" si="0">L3-B3</f>
+        <v>333125</v>
+      </c>
+      <c r="N3" s="6">
+        <v>52423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -770,8 +965,15 @@
       <c r="L4" s="6">
         <v>713985</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M4" s="6">
+        <f t="shared" si="0"/>
+        <v>86022</v>
+      </c>
+      <c r="N4" s="6">
+        <v>656425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -808,8 +1010,15 @@
       <c r="L5" s="6">
         <v>6413737</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M5" s="6">
+        <f t="shared" si="0"/>
+        <v>1253151</v>
+      </c>
+      <c r="N5" s="6">
+        <v>114006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -846,8 +1055,15 @@
       <c r="L6" s="6">
         <v>2921606</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M6" s="6">
+        <f t="shared" si="0"/>
+        <v>243018</v>
+      </c>
+      <c r="N6" s="6">
+        <v>53182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -884,8 +1100,15 @@
       <c r="L7" s="6">
         <v>37349363</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M7" s="6">
+        <f t="shared" si="0"/>
+        <v>3361386</v>
+      </c>
+      <c r="N7" s="6">
+        <v>163707</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -922,8 +1145,15 @@
       <c r="L8" s="6">
         <v>5049071</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M8" s="6">
+        <f t="shared" si="0"/>
+        <v>722150</v>
+      </c>
+      <c r="N8" s="6">
+        <v>104100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -960,8 +1190,15 @@
       <c r="L9" s="6">
         <v>3577073</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M9" s="6">
+        <f t="shared" si="0"/>
+        <v>165296</v>
+      </c>
+      <c r="N9" s="6">
+        <v>5544</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -998,8 +1235,15 @@
       <c r="L10" s="6">
         <v>899769</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M10" s="6">
+        <f t="shared" si="0"/>
+        <v>113396</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1036,8 +1280,15 @@
       <c r="L11" s="6">
         <v>604453</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M11" s="6">
+        <f t="shared" si="0"/>
+        <v>32407</v>
+      </c>
+      <c r="N11" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1074,8 +1325,15 @@
       <c r="L12" s="6">
         <v>18843326</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M12" s="6">
+        <f t="shared" si="0"/>
+        <v>2795811</v>
+      </c>
+      <c r="N12" s="6">
+        <v>65758</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1112,8 +1370,15 @@
       <c r="L13" s="6">
         <v>9712587</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M13" s="6">
+        <f t="shared" si="0"/>
+        <v>1485284</v>
+      </c>
+      <c r="N13" s="6">
+        <v>59441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1150,8 +1415,15 @@
       <c r="L14" s="6">
         <v>1363621</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M14" s="6">
+        <f t="shared" si="0"/>
+        <v>150102</v>
+      </c>
+      <c r="N14" s="6">
+        <v>10932</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1188,8 +1460,15 @@
       <c r="L15" s="6">
         <v>1571450</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M15" s="6">
+        <f t="shared" si="0"/>
+        <v>272020</v>
+      </c>
+      <c r="N15" s="6">
+        <v>83574</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -1226,8 +1505,15 @@
       <c r="L16" s="6">
         <v>12843166</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M16" s="6">
+        <f t="shared" si="0"/>
+        <v>409005</v>
+      </c>
+      <c r="N16" s="6">
+        <v>57918</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1264,8 +1550,15 @@
       <c r="L17" s="6">
         <v>6490621</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M17" s="6">
+        <f t="shared" si="0"/>
+        <v>398755</v>
+      </c>
+      <c r="N17" s="6">
+        <v>36420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1302,8 +1595,15 @@
       <c r="L18" s="6">
         <v>3049883</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M18" s="6">
+        <f t="shared" si="0"/>
+        <v>120816</v>
+      </c>
+      <c r="N18" s="6">
+        <v>56276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1340,8 +1640,15 @@
       <c r="L19" s="6">
         <v>2859169</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M19" s="6">
+        <f t="shared" si="0"/>
+        <v>165488</v>
+      </c>
+      <c r="N19" s="6">
+        <v>82282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1378,8 +1685,15 @@
       <c r="L20" s="6">
         <v>4346266</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M20" s="6">
+        <f t="shared" si="0"/>
+        <v>297245</v>
+      </c>
+      <c r="N20" s="6">
+        <v>40411</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1416,8 +1730,15 @@
       <c r="L21" s="6">
         <v>4544228</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M21" s="6">
+        <f t="shared" si="0"/>
+        <v>72343</v>
+      </c>
+      <c r="N21" s="6">
+        <v>51843</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1454,8 +1775,15 @@
       <c r="L22" s="6">
         <v>1327567</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M22" s="6">
+        <f t="shared" si="0"/>
+        <v>50495</v>
+      </c>
+      <c r="N22" s="6">
+        <v>35387</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1492,8 +1820,15 @@
       <c r="L23" s="6">
         <v>5785982</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M23" s="6">
+        <f t="shared" si="0"/>
+        <v>474948</v>
+      </c>
+      <c r="N23" s="6">
+        <v>12407</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1530,8 +1865,15 @@
       <c r="L24" s="6">
         <v>6557254</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M24" s="6">
+        <f t="shared" si="0"/>
+        <v>196150</v>
+      </c>
+      <c r="N24" s="6">
+        <v>10555</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1568,8 +1910,15 @@
       <c r="L25" s="6">
         <v>9877574</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M25" s="6">
+        <f t="shared" si="0"/>
+        <v>-74876</v>
+      </c>
+      <c r="N25" s="6">
+        <v>96810</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
@@ -1606,8 +1955,15 @@
       <c r="L26" s="6">
         <v>5310584</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M26" s="6">
+        <f t="shared" si="0"/>
+        <v>376892</v>
+      </c>
+      <c r="N26" s="6">
+        <v>86943</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1644,8 +2000,15 @@
       <c r="L27" s="6">
         <v>2970036</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M27" s="6">
+        <f t="shared" si="0"/>
+        <v>121683</v>
+      </c>
+      <c r="N27" s="6">
+        <v>48434</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1682,8 +2045,15 @@
       <c r="L28" s="6">
         <v>5996231</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M28" s="6">
+        <f t="shared" si="0"/>
+        <v>388946</v>
+      </c>
+      <c r="N28" s="6">
+        <v>69709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
@@ -1720,8 +2090,15 @@
       <c r="L29" s="6">
         <v>990898</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M29" s="6">
+        <f t="shared" si="0"/>
+        <v>87125</v>
+      </c>
+      <c r="N29" s="6">
+        <v>147046</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
@@ -1758,8 +2135,15 @@
       <c r="L30" s="6">
         <v>1830429</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M30" s="6">
+        <f t="shared" si="0"/>
+        <v>116609</v>
+      </c>
+      <c r="N30" s="6">
+        <v>77358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -1796,8 +2180,15 @@
       <c r="L31" s="6">
         <v>2704642</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M31" s="6">
+        <f t="shared" si="0"/>
+        <v>685901</v>
+      </c>
+      <c r="N31" s="6">
+        <v>110567</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
@@ -1834,8 +2225,15 @@
       <c r="L32" s="6">
         <v>1316759</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M32" s="6">
+        <f t="shared" si="0"/>
+        <v>76877</v>
+      </c>
+      <c r="N32" s="6">
+        <v>9351</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1872,8 +2270,15 @@
       <c r="L33" s="6">
         <v>8801624</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M33" s="6">
+        <f t="shared" si="0"/>
+        <v>371003</v>
+      </c>
+      <c r="N33" s="6">
+        <v>8722</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
@@ -1910,8 +2315,15 @@
       <c r="L34" s="6">
         <v>2065932</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M34" s="6">
+        <f t="shared" si="0"/>
+        <v>244728</v>
+      </c>
+      <c r="N34" s="6">
+        <v>121593</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
@@ -1948,8 +2360,15 @@
       <c r="L35" s="6">
         <v>19392283</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M35" s="6">
+        <f t="shared" si="0"/>
+        <v>390503</v>
+      </c>
+      <c r="N35" s="6">
+        <v>54475</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
@@ -1986,8 +2405,15 @@
       <c r="L36" s="6">
         <v>9561558</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M36" s="6">
+        <f t="shared" si="0"/>
+        <v>1479944</v>
+      </c>
+      <c r="N36" s="6">
+        <v>53821</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
@@ -2024,8 +2450,15 @@
       <c r="L37" s="6">
         <v>674499</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M37" s="6">
+        <f t="shared" si="0"/>
+        <v>32476</v>
+      </c>
+      <c r="N37" s="6">
+        <v>70704</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
@@ -2062,8 +2495,15 @@
       <c r="L38" s="6">
         <v>11536182</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M38" s="6">
+        <f t="shared" si="0"/>
+        <v>172639</v>
+      </c>
+      <c r="N38" s="6">
+        <v>44828</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
@@ -2100,8 +2540,15 @@
       <c r="L39" s="6">
         <v>3761702</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M39" s="6">
+        <f t="shared" si="0"/>
+        <v>307337</v>
+      </c>
+      <c r="N39" s="6">
+        <v>69903</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
@@ -2138,8 +2585,15 @@
       <c r="L40" s="6">
         <v>3838957</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M40" s="6">
+        <f t="shared" si="0"/>
+        <v>409249</v>
+      </c>
+      <c r="N40" s="6">
+        <v>98386</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -2176,8 +2630,15 @@
       <c r="L41" s="6">
         <v>12709630</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M41" s="6">
+        <f t="shared" si="0"/>
+        <v>425457</v>
+      </c>
+      <c r="N41" s="6">
+        <v>46058</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="5" t="s">
         <v>41</v>
       </c>
@@ -2214,8 +2675,15 @@
       <c r="L42" s="6">
         <v>1052886</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M42" s="6">
+        <f t="shared" si="0"/>
+        <v>2618</v>
+      </c>
+      <c r="N42" s="6">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -2252,8 +2720,15 @@
       <c r="L43" s="6">
         <v>4636312</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M43" s="6">
+        <f t="shared" si="0"/>
+        <v>612089</v>
+      </c>
+      <c r="N43" s="6">
+        <v>32007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="5" t="s">
         <v>43</v>
       </c>
@@ -2290,8 +2765,15 @@
       <c r="L44" s="6">
         <v>816463</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M44" s="6">
+        <f t="shared" si="0"/>
+        <v>60619</v>
+      </c>
+      <c r="N44" s="6">
+        <v>77121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="5" t="s">
         <v>44</v>
       </c>
@@ -2328,8 +2810,15 @@
       <c r="L45" s="6">
         <v>6356897</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M45" s="6">
+        <f t="shared" si="0"/>
+        <v>653178</v>
+      </c>
+      <c r="N45" s="6">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
@@ -2366,8 +2855,15 @@
       <c r="L46" s="6">
         <v>25257114</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M46" s="6">
+        <f t="shared" si="0"/>
+        <v>4312615</v>
+      </c>
+      <c r="N46" s="6">
+        <v>268601</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
@@ -2404,8 +2900,15 @@
       <c r="L47" s="6">
         <v>2776469</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M47" s="6">
+        <f t="shared" si="0"/>
+        <v>531967</v>
+      </c>
+      <c r="N47" s="6">
+        <v>84904</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
@@ -2442,8 +2945,15 @@
       <c r="L48" s="6">
         <v>625960</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M48" s="6">
+        <f t="shared" si="0"/>
+        <v>16342</v>
+      </c>
+      <c r="N48" s="6">
+        <v>9615</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
@@ -2480,8 +2990,15 @@
       <c r="L49" s="6">
         <v>8024617</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M49" s="6">
+        <f t="shared" si="0"/>
+        <v>918800</v>
+      </c>
+      <c r="N49" s="6">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="5" t="s">
         <v>49</v>
       </c>
@@ -2518,8 +3035,15 @@
       <c r="L50" s="6">
         <v>6744496</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M50" s="6">
+        <f t="shared" si="0"/>
+        <v>833984</v>
+      </c>
+      <c r="N50" s="6">
+        <v>71303</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
@@ -2556,8 +3080,15 @@
       <c r="L51" s="6">
         <v>1853973</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M51" s="6">
+        <f t="shared" si="0"/>
+        <v>46952</v>
+      </c>
+      <c r="N51" s="6">
+        <v>24231</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="5" t="s">
         <v>51</v>
       </c>
@@ -2594,8 +3125,15 @@
       <c r="L52" s="6">
         <v>5691047</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M52" s="6">
+        <f t="shared" si="0"/>
+        <v>317048</v>
+      </c>
+      <c r="N52" s="6">
+        <v>65503</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="5" t="s">
         <v>52</v>
       </c>
@@ -2631,9 +3169,300 @@
       </c>
       <c r="L53" s="6">
         <v>564460</v>
+      </c>
+      <c r="M53" s="6">
+        <f t="shared" si="0"/>
+        <v>70160</v>
+      </c>
+      <c r="N53" s="6">
+        <v>97818</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2155D6-2756-4098-B203-D9298A49B5E6}">
+  <dimension ref="A1:A53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection sqref="A1:A53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="17.9453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>